<commit_message>
Nu echt finale versie met asymmetrische brug
</commit_message>
<xml_diff>
--- a/6tuien.xlsx
+++ b/6tuien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArnoD\Documents\GitHub\brug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B46835-0BA8-474D-B74C-2D9F42A36DA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90A957A-B826-4C69-A532-6411DC73C9BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="756" windowWidth="12960" windowHeight="8964" xr2:uid="{54D56187-4AD6-4CEE-93BE-48D0436DC814}"/>
+    <workbookView xWindow="1044" yWindow="1800" windowWidth="12960" windowHeight="8964" xr2:uid="{00807199-5EEE-4595-BB17-DF9591AA9198}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB2835F-7A55-4F06-BCAB-C38686A9EBD3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4FD7D9-B0A1-42AA-A853-EFE2DCDAC247}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -428,78 +428,78 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="B2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="C2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="D2">
-        <v>-419.55057417440332</v>
+        <v>596.28479399994387</v>
       </c>
       <c r="E2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="F2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="G2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="H2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="I2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="J2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="K2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
       <c r="L2">
-        <v>-104.88764354360083</v>
+        <v>149.07119849998597</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="B3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="C3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="D3">
-        <v>-323.90056063390881</v>
+        <v>533.33333333333326</v>
       </c>
       <c r="E3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="F3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="G3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="H3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="I3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="J3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="K3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
       <c r="L3">
-        <v>-80.975140158477203</v>
+        <v>133.33333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>